<commit_message>
updated or removed excel files so that remaining ones can be imported
</commit_message>
<xml_diff>
--- a/MPTrx/_IDP.xlsx
+++ b/MPTrx/_IDP.xlsx
@@ -128,9 +128,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>[Role,]</t>
-  </si>
-  <si>
     <t>tinus.otto@tno.nl</t>
   </si>
   <si>
@@ -240,6 +237,9 @@
   </si>
   <si>
     <t>accAutoLoginReq</t>
+  </si>
+  <si>
+    <t>Role</t>
   </si>
 </sst>
 </file>
@@ -676,7 +676,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,7 +728,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -744,7 +744,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="3"/>
@@ -760,7 +760,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="3"/>
@@ -773,10 +773,10 @@
         <v>Overheid</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="3"/>
@@ -827,7 +827,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>15</v>
@@ -838,72 +838,72 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -926,7 +926,7 @@
         <v>22</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -946,7 +946,7 @@
         <v>5</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>23</v>
@@ -954,16 +954,16 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="D22" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>8</v>
@@ -975,16 +975,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="D23" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
@@ -992,16 +992,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>1</v>
@@ -1009,93 +1009,93 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MPTrx - revised, has debug interface, and is ready for further testing
</commit_message>
<xml_diff>
--- a/MPTrx/_IDP.xlsx
+++ b/MPTrx/_IDP.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3008DFB3-17C8-4DBB-B7FC-E886E03AE1BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200B3946-5BF5-460F-B685-DEDBA4593351}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="703" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-46188" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="703" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SIAM" sheetId="18" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="85">
   <si>
     <t>PGGM</t>
   </si>
@@ -299,6 +299,21 @@
   </si>
   <si>
     <t>PersonRef</t>
+  </si>
+  <si>
+    <t>AccountMgr</t>
+  </si>
+  <si>
+    <t>PersonMgr</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>OrganizationMgr</t>
+  </si>
+  <si>
+    <t>ExcelImporter</t>
   </si>
 </sst>
 </file>
@@ -803,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD19"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1291,41 +1306,77 @@
         <f>$A31</f>
         <v>Acc_tinus.otto@tno.nl</v>
       </c>
+      <c r="C31" s="4" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="str">
         <f t="shared" ref="A32:A37" si="3">$A23</f>
         <v>Acc_polisadm@pggm.nl</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C32" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="str">
         <f t="shared" si="3"/>
         <v>Acc_rijkdw@rdw.nl</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C33" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="str">
         <f t="shared" si="3"/>
         <v>Acc_digid@overheid.nl</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C34" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="str">
         <f t="shared" si="3"/>
         <v>Acc_cs12345@gmail.com</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C35" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="str">
         <f t="shared" si="3"/>
         <v>Acc_d.rijder@gmail.com</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C36" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="str">
         <f t="shared" si="3"/>
         <v/>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>